<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@b946abfe6682e48c03cce8508078d86cbbabb57a 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-research-data-date-of-birth-method-vs.xlsx
+++ b/ValueSet-research-data-date-of-birth-method-vs.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-28T00:06:22+00:00</t>
+    <t>2025-02-07T15:45:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -102,7 +102,7 @@
     <t>System URI</t>
   </si>
   <si>
-    <t>http://terminology.hl7.org/CodeSystem/title-type</t>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/CodeSystem/research-data-date-of-birth-method</t>
   </si>
 </sst>
 </file>

</xml_diff>